<commit_message>
josh messed with game code and added dist2steps
</commit_message>
<xml_diff>
--- a/mechanical/drive step info.xlsx
+++ b/mechanical/drive step info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joshua\Documents\School\2018-19\Spring\ECE 4990-001        IEEE Robotics\astrohub\mechanical\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BE3FC22E-6E73-4E3E-B86A-2291DF874EF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A61C8F-B64A-4F9B-A4A2-9D431F60836E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="4215" windowWidth="8685" windowHeight="11385" xr2:uid="{70850FC6-F549-465F-ACFC-63FEA5DF99C3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>STEPS</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>TURN</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>step/dist</t>
   </si>
 </sst>
 </file>
@@ -415,57 +421,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA0C3CE-82CC-4030-A443-03A121DDB830}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>900</v>
       </c>
       <c r="B3">
         <v>84.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">A3/B3</f>
+        <v>10.650887573964496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>450</v>
       </c>
       <c r="B4">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>10.714285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>225</v>
       </c>
       <c r="B5">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10.465116279069768</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <f>AVERAGE(D3:D5,D9:D11)</f>
+        <v>10.568326154996846</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -473,31 +503,43 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>900</v>
       </c>
       <c r="B9">
         <v>85.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f>A9/B9</f>
+        <v>10.526315789473685</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>450</v>
       </c>
       <c r="B10">
         <v>42.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <f t="shared" ref="D10:D11" si="1">A10/B10</f>
+        <v>10.588235294117647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>225</v>
       </c>
       <c r="B11">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>10.465116279069768</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -505,7 +547,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -515,8 +557,11 @@
       <c r="C14" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>900</v>
       </c>
@@ -531,7 +576,7 @@
         <v>0.18124999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>450</v>
       </c>
@@ -545,8 +590,12 @@
         <f>C16/B16</f>
         <v>0.20338983050847459</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f>A16/B16</f>
+        <v>15.254237288135593</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>225</v>
       </c>
@@ -560,16 +609,29 @@
         <f>C17/B17</f>
         <v>0.16129032258064516</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f>A17/B17</f>
+        <v>14.516129032258064</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
       <c r="C19">
         <v>2500</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <f>AVERAGE(J16:J17,J22:J23)</f>
+        <v>14.473841580098414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -580,7 +642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>900</v>
       </c>
@@ -598,7 +660,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>450</v>
       </c>
@@ -612,8 +674,12 @@
         <f>C22/B22</f>
         <v>0.15625</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f>A22/B22</f>
+        <v>14.0625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>225</v>
       </c>
@@ -630,18 +696,22 @@
       <c r="G23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f>A23/B23</f>
+        <v>14.0625</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>270</v>
       </c>

</xml_diff>